<commit_message>
more values for daan! yay
</commit_message>
<xml_diff>
--- a/Added Mass, Damping, Stiffness.xlsx
+++ b/Added Mass, Damping, Stiffness.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\floating_wind_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D53663-D5B1-45FB-8F04-486AA2F1FAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F1C71A-B150-489D-80DA-35B1D8BC5C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7F7944D8-6F0D-44EF-A699-D3CC7E9BF926}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="23">
   <si>
     <t>spar_125</t>
   </si>
@@ -80,6 +80,30 @@
   </si>
   <si>
     <t>4.1 rad/s</t>
+  </si>
+  <si>
+    <t>spar_1_075</t>
+  </si>
+  <si>
+    <t>d1 = 0.075m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 = 0.12m </t>
+  </si>
+  <si>
+    <t>d2 = 0.365m</t>
+  </si>
+  <si>
+    <t>h2 = 0.001</t>
+  </si>
+  <si>
+    <t>spar_2_01</t>
+  </si>
+  <si>
+    <t>d1 = 0.1m</t>
+  </si>
+  <si>
+    <t>d2 = 0.446m</t>
   </si>
 </sst>
 </file>
@@ -118,10 +142,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48AA4CE-07F3-4354-9B72-B22D39F08613}">
-  <dimension ref="A2:W10"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,6 +967,865 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" t="s">
+        <v>13</v>
+      </c>
+      <c r="S15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" t="s">
+        <v>5</v>
+      </c>
+      <c r="U17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V17" t="s">
+        <v>7</v>
+      </c>
+      <c r="W17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.399</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-6.36</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>0.79453726829268301</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>-2.4918517073170698</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.399</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6.3650000000000002</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0.79461053658536596</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>2.4918146341463401</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>17.48</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>172.9</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>5</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>-11.2984682926829</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-1.97</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>-3.2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>6</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>-0.25415570731707299</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>-0.80162907317073195</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.9670000000000001</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>-3.2</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>7</v>
+      </c>
+      <c r="R22">
+        <v>0.25411717073170698</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22" s="2">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>-0.80159795121951205</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>6</v>
+      </c>
+      <c r="N31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2.609</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-0.11</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2.609</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.111</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2.3620000000000001</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>307.8</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>25.82</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-3.2000000000000002E-8</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>-4.18</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-32.9</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>25.82</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>-4.18</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2.5000000000000002E-16</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test of spar vs barge
</commit_message>
<xml_diff>
--- a/Added Mass, Damping, Stiffness.xlsx
+++ b/Added Mass, Damping, Stiffness.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\floating_wind_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E18A73-B8FC-47B3-A3DD-BE09FE61F4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217949DA-61C9-45E7-A23C-1DB34F3B1470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7F7944D8-6F0D-44EF-A699-D3CC7E9BF926}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7F7944D8-6F0D-44EF-A699-D3CC7E9BF926}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="39">
   <si>
     <t>spar_125</t>
   </si>
@@ -138,11 +139,29 @@
   <si>
     <t>d2 = 0.68m</t>
   </si>
+  <si>
+    <t>spar_eqiv</t>
+  </si>
+  <si>
+    <t>barge_equiv</t>
+  </si>
+  <si>
+    <t>semisub_equiv</t>
+  </si>
+  <si>
+    <t>times 4 for semi-sub</t>
+  </si>
+  <si>
+    <t>HYDROSTATIC STIFFNESS MATRICES</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,10 +197,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48AA4CE-07F3-4354-9B72-B22D39F08613}">
   <dimension ref="A2:X95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="G67" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3762,4 +3785,700 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D951921-A7D4-4610-9496-073A04A7CE59}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>110.8</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1231</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>9.3059999999999992</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>9.3059999999999992</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>110.8</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>D18*4</f>
+        <v>443.2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:N18" si="0">E18*4</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ref="L19:L20" si="1">D19*4</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ref="M19:M20" si="2">E19*4</f>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ref="N19:N20" si="3">F19*4</f>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="3"/>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>